<commit_message>
lan 25 gan hoan thien man 2
</commit_message>
<xml_diff>
--- a/MAP/map_level2.xlsx
+++ b/MAP/map_level2.xlsx
@@ -694,7 +694,7 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="29">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -776,13 +776,6 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -979,25 +972,25 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="19"/>
-      <tableStyleElement type="headerRow" dxfId="18"/>
-      <tableStyleElement type="totalRow" dxfId="17"/>
-      <tableStyleElement type="firstColumn" dxfId="16"/>
-      <tableStyleElement type="lastColumn" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="wholeTable" dxfId="18"/>
+      <tableStyleElement type="headerRow" dxfId="17"/>
+      <tableStyleElement type="totalRow" dxfId="16"/>
+      <tableStyleElement type="firstColumn" dxfId="15"/>
+      <tableStyleElement type="lastColumn" dxfId="14"/>
+      <tableStyleElement type="firstRowStripe" dxfId="13"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="12"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="29"/>
-      <tableStyleElement type="totalRow" dxfId="28"/>
-      <tableStyleElement type="firstRowStripe" dxfId="27"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="26"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="25"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="24"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="23"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="22"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="21"/>
-      <tableStyleElement type="pageFieldValues" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="28"/>
+      <tableStyleElement type="totalRow" dxfId="27"/>
+      <tableStyleElement type="firstRowStripe" dxfId="26"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="25"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="24"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="23"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="22"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="21"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="20"/>
+      <tableStyleElement type="pageFieldValues" dxfId="19"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1268,8 +1261,8 @@
   <sheetPr/>
   <dimension ref="A1:EJ45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BS19" workbookViewId="0">
-      <selection activeCell="DU52" sqref="DU52"/>
+    <sheetView tabSelected="1" topLeftCell="BS31" workbookViewId="0">
+      <selection activeCell="DO53" sqref="DO53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.62857142857143" defaultRowHeight="15"/>
@@ -1312,8 +1305,8 @@
     <col min="99" max="99" width="3.57142857142857" style="1"/>
     <col min="100" max="100" width="2.57142857142857" style="1" customWidth="1"/>
     <col min="101" max="110" width="3.57142857142857" style="1"/>
-    <col min="111" max="112" width="2.62857142857143" style="1"/>
-    <col min="113" max="113" width="3.57142857142857" style="1"/>
+    <col min="111" max="111" width="2.62857142857143" style="1"/>
+    <col min="112" max="113" width="3.57142857142857" style="1"/>
     <col min="114" max="120" width="2.62857142857143" style="1"/>
     <col min="121" max="128" width="3.57142857142857" style="1"/>
     <col min="129" max="134" width="2.62857142857143" style="1"/>
@@ -14813,7 +14806,7 @@
         <v>0</v>
       </c>
       <c r="EG32" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="EH32" s="1">
         <v>5</v>
@@ -17267,10 +17260,10 @@
         <v>0</v>
       </c>
       <c r="DG38" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DH38" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DI38" s="1">
         <v>0</v>
@@ -18515,16 +18508,16 @@
         <v>0</v>
       </c>
       <c r="DA41" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DB41" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DC41" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DD41" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="DE41" s="1">
         <v>0</v>
@@ -18943,10 +18936,10 @@
         <v>0</v>
       </c>
       <c r="DC42" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="DD42" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="DE42" s="1">
         <v>0</v>
@@ -20388,7 +20381,7 @@
     <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
       <formula>15</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
lan 25 man 3
</commit_message>
<xml_diff>
--- a/MAP/map_level2.xlsx
+++ b/MAP/map_level2.xlsx
@@ -1261,8 +1261,8 @@
   <sheetPr/>
   <dimension ref="A1:EJ45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BS31" workbookViewId="0">
-      <selection activeCell="DO53" sqref="DO53"/>
+    <sheetView tabSelected="1" topLeftCell="BS22" workbookViewId="0">
+      <selection activeCell="DV47" sqref="DV47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.62857142857143" defaultRowHeight="15"/>
@@ -17260,10 +17260,10 @@
         <v>0</v>
       </c>
       <c r="DG38" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="DH38" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="DI38" s="1">
         <v>0</v>

</xml_diff>